<commit_message>
Install kbd dll on reboot when in use
</commit_message>
<xml_diff>
--- a/images/layouts.xlsx
+++ b/images/layouts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thierry.Lelegard\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lelegard\Documents\winkbdlayouts\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0879F93B-4ABB-4554-B69F-DBDE30C5DC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35743BBE-918C-4A1D-8CE0-5851C4D69D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="4695" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{74A816CA-6688-4E74-BB41-54318C953D2B}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21330" windowHeight="12645" activeTab="1" xr2:uid="{74A816CA-6688-4E74-BB41-54318C953D2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Scan Codes" sheetId="2" r:id="rId1"/>
@@ -612,30 +612,6 @@
 à @</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">° </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-) ]</t>
-    </r>
-  </si>
-  <si>
     <t>+ ≈
 = }</t>
   </si>
@@ -1129,72 +1105,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">W </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-w </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>_</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">X </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
-x </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>_</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">C </t>
     </r>
     <r>
@@ -1282,6 +1192,18 @@
       <t xml:space="preserve">
 b ß</t>
     </r>
+  </si>
+  <si>
+    <t>° π
+) ]</t>
+  </si>
+  <si>
+    <t>W Φ
+w φ</t>
+  </si>
+  <si>
+    <t>X Ψ
+x ψ</t>
   </si>
 </sst>
 </file>
@@ -1459,100 +1381,100 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1883,553 +1805,635 @@
   <sheetData>
     <row r="1" spans="2:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="21" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="21" t="s">
+      <c r="L2" s="9"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21" t="s">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21" t="s">
+      <c r="S2" s="9"/>
+      <c r="T2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="21"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="21" t="s">
+      <c r="U2" s="9"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21" t="s">
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21" t="s">
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21" t="s">
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="23" t="s">
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AH2" s="24"/>
-      <c r="AI2" s="23" t="s">
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="23" t="s">
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4"/>
     </row>
     <row r="3" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="22"/>
-      <c r="Z3" s="22"/>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="22"/>
-      <c r="AE3" s="22"/>
-      <c r="AF3" s="22"/>
-      <c r="AG3" s="22"/>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="22"/>
-      <c r="AJ3" s="22"/>
-      <c r="AK3" s="22"/>
-      <c r="AL3" s="22"/>
-      <c r="AM3" s="22"/>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="22"/>
-      <c r="AQ3" s="22"/>
-      <c r="AR3" s="22"/>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="22"/>
-      <c r="AU3" s="22"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4"/>
+      <c r="AT3" s="4"/>
+      <c r="AU3" s="4"/>
     </row>
     <row r="4" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21" t="s">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21" t="s">
+      <c r="M4" s="9"/>
+      <c r="N4" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21" t="s">
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21" t="s">
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21" t="s">
+      <c r="S4" s="9"/>
+      <c r="T4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21" t="s">
+      <c r="U4" s="9"/>
+      <c r="V4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21" t="s">
+      <c r="W4" s="9"/>
+      <c r="X4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21" t="s">
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21" t="s">
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="21"/>
-      <c r="AE4" s="21"/>
-      <c r="AF4" s="22"/>
-      <c r="AG4" s="23" t="s">
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="23" t="s">
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AJ4" s="24"/>
-      <c r="AK4" s="23" t="s">
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="21" t="s">
+      <c r="AL4" s="7"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AO4" s="21"/>
-      <c r="AP4" s="21" t="s">
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="AQ4" s="21"/>
-      <c r="AR4" s="21" t="s">
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AS4" s="21"/>
-      <c r="AT4" s="21" t="s">
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AU4" s="21"/>
+      <c r="AU4" s="9"/>
     </row>
     <row r="5" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26" t="s">
+      <c r="L5" s="15"/>
+      <c r="M5" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26" t="s">
+      <c r="N5" s="15"/>
+      <c r="O5" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26" t="s">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26" t="s">
+      <c r="R5" s="15"/>
+      <c r="S5" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26" t="s">
+      <c r="T5" s="15"/>
+      <c r="U5" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26" t="s">
+      <c r="V5" s="15"/>
+      <c r="W5" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26" t="s">
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26" t="s">
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26" t="s">
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="22"/>
-      <c r="AG5" s="23" t="s">
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="23" t="s">
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="23" t="s">
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="22"/>
-      <c r="AN5" s="21" t="s">
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AO5" s="21"/>
-      <c r="AP5" s="21" t="s">
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="AQ5" s="21"/>
-      <c r="AR5" s="21" t="s">
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AS5" s="21"/>
-      <c r="AT5" s="27" t="s">
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="AU5" s="28"/>
+      <c r="AU5" s="11"/>
     </row>
     <row r="6" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21" t="s">
+      <c r="O6" s="9"/>
+      <c r="P6" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21" t="s">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21" t="s">
+      <c r="S6" s="9"/>
+      <c r="T6" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21" t="s">
+      <c r="U6" s="9"/>
+      <c r="V6" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21" t="s">
+      <c r="W6" s="9"/>
+      <c r="X6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21" t="s">
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21" t="s">
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="22"/>
-      <c r="AI6" s="22"/>
-      <c r="AJ6" s="22"/>
-      <c r="AK6" s="22"/>
-      <c r="AL6" s="22"/>
-      <c r="AM6" s="22"/>
-      <c r="AN6" s="21" t="s">
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="4"/>
+      <c r="AG6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="AO6" s="21"/>
-      <c r="AP6" s="21" t="s">
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="AQ6" s="21"/>
-      <c r="AR6" s="21" t="s">
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AS6" s="21"/>
-      <c r="AT6" s="30"/>
-      <c r="AU6" s="31"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="12"/>
+      <c r="AU6" s="13"/>
     </row>
     <row r="7" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="23" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="23" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="23" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="23" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="23" t="s">
+      <c r="L7" s="7"/>
+      <c r="M7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="24"/>
-      <c r="O7" s="23" t="s">
+      <c r="N7" s="7"/>
+      <c r="O7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="23" t="s">
+      <c r="P7" s="7"/>
+      <c r="Q7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="R7" s="24"/>
-      <c r="S7" s="23" t="s">
+      <c r="R7" s="7"/>
+      <c r="S7" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="T7" s="24"/>
-      <c r="U7" s="23" t="s">
+      <c r="T7" s="7"/>
+      <c r="U7" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="V7" s="24"/>
-      <c r="W7" s="23" t="s">
+      <c r="V7" s="7"/>
+      <c r="W7" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="23" t="s">
+      <c r="X7" s="7"/>
+      <c r="Y7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="23" t="s">
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="32"/>
-      <c r="AD7" s="32"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="22"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="22"/>
-      <c r="AI7" s="21" t="s">
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="4"/>
+      <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
+      <c r="AI7" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="AJ7" s="21"/>
-      <c r="AK7" s="22"/>
-      <c r="AL7" s="22"/>
-      <c r="AM7" s="22"/>
-      <c r="AN7" s="21" t="s">
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
+      <c r="AN7" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AO7" s="21"/>
-      <c r="AP7" s="21" t="s">
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="AQ7" s="21"/>
-      <c r="AR7" s="21" t="s">
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="AS7" s="21"/>
-      <c r="AT7" s="27" t="s">
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="AU7" s="28"/>
+      <c r="AU7" s="11"/>
     </row>
     <row r="8" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="23" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="23" t="s">
+      <c r="F8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="23" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="23" t="s">
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="23" t="s">
+      <c r="U8" s="8"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="23" t="s">
+      <c r="X8" s="8"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="23" t="s">
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="AD8" s="32"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="22"/>
-      <c r="AG8" s="23" t="s">
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="4"/>
+      <c r="AG8" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="AH8" s="24"/>
-      <c r="AI8" s="23" t="s">
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="AJ8" s="24"/>
-      <c r="AK8" s="23" t="s">
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="AL8" s="24"/>
-      <c r="AM8" s="22"/>
-      <c r="AN8" s="23" t="s">
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="AO8" s="32"/>
-      <c r="AP8" s="32"/>
-      <c r="AQ8" s="24"/>
-      <c r="AR8" s="21" t="s">
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="AS8" s="21"/>
-      <c r="AT8" s="30"/>
-      <c r="AU8" s="31"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="12"/>
+      <c r="AU8" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AB4:AE4"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AT5:AU6"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AN6:AO6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AR6:AS6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="AI8:AJ8"/>
     <mergeCell ref="AK8:AL8"/>
     <mergeCell ref="AN8:AQ8"/>
@@ -2454,88 +2458,6 @@
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AN6:AO6"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AR6:AS6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AT5:AU6"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AE5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AB4:AE4"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2552,7 +2474,9 @@
   </sheetPr>
   <dimension ref="B1:AU8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2561,500 +2485,540 @@
   <sheetData>
     <row r="1" spans="2:47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="J2" s="16"/>
+      <c r="K2" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="9" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9" t="s">
+      <c r="O2" s="16"/>
+      <c r="P2" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9" t="s">
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="s">
+      <c r="S2" s="16"/>
+      <c r="T2" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="9" t="s">
+      <c r="U2" s="16"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9" t="s">
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9" t="s">
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9" t="s">
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="14" t="s">
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="14" t="s">
+      <c r="AH2" s="23"/>
+      <c r="AI2" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="10" t="s">
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="AL2" s="12"/>
+      <c r="AL2" s="23"/>
     </row>
     <row r="3" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="29"/>
+      <c r="H4" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="7" t="s">
+      <c r="I4" s="29"/>
+      <c r="J4" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="29"/>
+      <c r="L4" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="7" t="s">
+      <c r="M4" s="29"/>
+      <c r="N4" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="7" t="s">
+      <c r="O4" s="29"/>
+      <c r="P4" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="7" t="s">
+      <c r="Q4" s="29"/>
+      <c r="R4" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="7" t="s">
+      <c r="S4" s="29"/>
+      <c r="T4" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="U4" s="3"/>
-      <c r="V4" s="7" t="s">
+      <c r="U4" s="29"/>
+      <c r="V4" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="7" t="s">
+      <c r="W4" s="29"/>
+      <c r="X4" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="9" t="s">
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AG4" s="10" t="s">
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AG4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="10" t="s">
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AJ4" s="12"/>
-      <c r="AK4" s="14" t="s">
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AL4" s="12"/>
-      <c r="AN4" s="15" t="s">
+      <c r="AL4" s="23"/>
+      <c r="AN4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="9" t="s">
+      <c r="AO4" s="16"/>
+      <c r="AP4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="9" t="s">
+      <c r="AQ4" s="16"/>
+      <c r="AR4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="AS4" s="9"/>
-      <c r="AT4" s="9" t="s">
+      <c r="AS4" s="16"/>
+      <c r="AT4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AU4" s="9"/>
+      <c r="AU4" s="16"/>
     </row>
     <row r="5" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="34" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="34" t="s">
+      <c r="J5" s="32"/>
+      <c r="K5" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="34" t="s">
+      <c r="L5" s="32"/>
+      <c r="M5" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="34" t="s">
+      <c r="N5" s="32"/>
+      <c r="O5" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="34" t="s">
+      <c r="P5" s="32"/>
+      <c r="Q5" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="34" t="s">
+      <c r="R5" s="32"/>
+      <c r="S5" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="34" t="s">
+      <c r="T5" s="32"/>
+      <c r="U5" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="34" t="s">
+      <c r="V5" s="32"/>
+      <c r="W5" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="V5" s="4"/>
-      <c r="W5" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="34" t="s">
+      <c r="X5" s="32"/>
+      <c r="Y5" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="8" t="s">
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AG5" s="10" t="s">
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AG5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="10" t="s">
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="14" t="s">
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AL5" s="12"/>
-      <c r="AN5" s="9">
+      <c r="AL5" s="23"/>
+      <c r="AN5" s="16">
         <v>7</v>
       </c>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9">
+      <c r="AO5" s="16"/>
+      <c r="AP5" s="16">
         <v>8</v>
       </c>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9">
+      <c r="AQ5" s="16"/>
+      <c r="AR5" s="16">
         <v>9</v>
       </c>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="16" t="s">
+      <c r="AS5" s="16"/>
+      <c r="AT5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AU5" s="17"/>
+      <c r="AU5" s="18"/>
     </row>
     <row r="6" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="7" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="29"/>
+      <c r="J6" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="29"/>
+      <c r="N6" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="29"/>
+      <c r="P6" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="29"/>
+      <c r="R6" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="7" t="s">
+      <c r="S6" s="29"/>
+      <c r="T6" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="7" t="s">
+      <c r="U6" s="29"/>
+      <c r="V6" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="U6" s="3"/>
-      <c r="V6" s="7" t="s">
+      <c r="W6" s="29"/>
+      <c r="X6" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="W6" s="3"/>
-      <c r="X6" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="7" t="s">
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AN6" s="9">
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="30"/>
+      <c r="AN6" s="16">
         <v>4</v>
       </c>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9">
+      <c r="AO6" s="16"/>
+      <c r="AP6" s="16">
         <v>5</v>
       </c>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9">
+      <c r="AQ6" s="16"/>
+      <c r="AR6" s="16">
         <v>6</v>
       </c>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="18"/>
-      <c r="AU6" s="19"/>
+      <c r="AS6" s="16"/>
+      <c r="AT6" s="19"/>
+      <c r="AU6" s="20"/>
     </row>
     <row r="7" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="13" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="L7" s="27"/>
+      <c r="M7" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="N7" s="27"/>
+      <c r="O7" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="T7" s="6"/>
-      <c r="U7" s="13" t="s">
+      <c r="R7" s="27"/>
+      <c r="S7" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="V7" s="6"/>
-      <c r="W7" s="13" t="s">
+      <c r="T7" s="27"/>
+      <c r="U7" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="13" t="s">
+      <c r="V7" s="27"/>
+      <c r="W7" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="10" t="s">
+      <c r="X7" s="27"/>
+      <c r="Y7" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="12"/>
-      <c r="AI7" s="9" t="s">
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="23"/>
+      <c r="AI7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AJ7" s="9"/>
-      <c r="AN7" s="9">
+      <c r="AJ7" s="16"/>
+      <c r="AN7" s="16">
         <v>1</v>
       </c>
-      <c r="AO7" s="9"/>
-      <c r="AP7" s="9">
+      <c r="AO7" s="16"/>
+      <c r="AP7" s="16">
         <v>2</v>
       </c>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="9">
+      <c r="AQ7" s="16"/>
+      <c r="AR7" s="16">
         <v>3</v>
       </c>
-      <c r="AS7" s="9"/>
-      <c r="AT7" s="16" t="s">
+      <c r="AS7" s="16"/>
+      <c r="AT7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="AU7" s="17"/>
+      <c r="AU7" s="18"/>
     </row>
     <row r="8" spans="2:47" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="10" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="10" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="10" t="s">
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="U8" s="11"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="10" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="10" t="s">
+      <c r="X8" s="22"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="10" t="s">
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="12"/>
-      <c r="AG8" s="10" t="s">
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="23"/>
+      <c r="AG8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="10" t="s">
+      <c r="AH8" s="23"/>
+      <c r="AI8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="AJ8" s="12"/>
-      <c r="AK8" s="10" t="s">
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="AL8" s="12"/>
-      <c r="AN8" s="10">
+      <c r="AL8" s="23"/>
+      <c r="AN8" s="21">
         <v>0</v>
       </c>
-      <c r="AO8" s="11"/>
-      <c r="AP8" s="11"/>
-      <c r="AQ8" s="12"/>
-      <c r="AR8" s="9" t="s">
+      <c r="AO8" s="22"/>
+      <c r="AP8" s="22"/>
+      <c r="AQ8" s="23"/>
+      <c r="AR8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AS8" s="9"/>
-      <c r="AT8" s="18"/>
-      <c r="AU8" s="19"/>
+      <c r="AS8" s="16"/>
+      <c r="AT8" s="19"/>
+      <c r="AU8" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="AR8:AS8"/>
-    <mergeCell ref="AT5:AU6"/>
-    <mergeCell ref="AT7:AU8"/>
-    <mergeCell ref="AN8:AQ8"/>
-    <mergeCell ref="AN6:AO6"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AR6:AS6"/>
-    <mergeCell ref="AN7:AO7"/>
-    <mergeCell ref="AP7:AQ7"/>
-    <mergeCell ref="AR7:AS7"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="AB4:AE4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AE5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="AC8:AE8"/>
+    <mergeCell ref="Z8:AB8"/>
+    <mergeCell ref="W8:Y8"/>
+    <mergeCell ref="T8:V8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
     <mergeCell ref="K8:S8"/>
     <mergeCell ref="AG8:AH8"/>
     <mergeCell ref="AI8:AJ8"/>
@@ -3069,77 +3033,37 @@
     <mergeCell ref="W7:X7"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="AA7:AE7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="AC8:AE8"/>
-    <mergeCell ref="Z8:AB8"/>
-    <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="T8:V8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="X6:Y6"/>
     <mergeCell ref="Z6:AA6"/>
     <mergeCell ref="AB6:AC6"/>
     <mergeCell ref="AD6:AE6"/>
     <mergeCell ref="T2:U2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AE5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="AB4:AE4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AR8:AS8"/>
+    <mergeCell ref="AT5:AU6"/>
+    <mergeCell ref="AT7:AU8"/>
+    <mergeCell ref="AN8:AQ8"/>
+    <mergeCell ref="AN6:AO6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AR6:AS6"/>
+    <mergeCell ref="AN7:AO7"/>
+    <mergeCell ref="AP7:AQ7"/>
+    <mergeCell ref="AR7:AS7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>